<commit_message>
Create Api and Fix Server Problem
</commit_message>
<xml_diff>
--- a/Project Details/ProjectDetails.xlsx
+++ b/Project Details/ProjectDetails.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="20055" windowHeight="9225" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="20052" windowHeight="9228" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Features" sheetId="1" r:id="rId1"/>
@@ -1078,14 +1078,14 @@
       <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
-    <row r="3" spans="1:21" ht="31.5">
+    <row r="3" spans="1:21" ht="31.2">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:21" ht="26.25">
+    <row r="5" spans="1:21" ht="25.8">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
@@ -1106,7 +1106,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:21" ht="26.25">
+    <row r="6" spans="1:21" ht="25.8">
       <c r="C6" s="5" t="s">
         <v>2</v>
       </c>
@@ -1118,7 +1118,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:21" ht="26.25">
+    <row r="7" spans="1:21" ht="25.8">
       <c r="C7" s="5" t="s">
         <v>3</v>
       </c>
@@ -1130,16 +1130,16 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:21" ht="23.25">
+    <row r="8" spans="1:21" ht="23.4">
       <c r="C8" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:21" ht="26.25">
+    <row r="9" spans="1:21" ht="25.8">
       <c r="Q9" s="6"/>
       <c r="U9" s="8"/>
     </row>
-    <row r="10" spans="1:21" ht="26.25">
+    <row r="10" spans="1:21" ht="25.8">
       <c r="A10" s="2" t="s">
         <v>11</v>
       </c>
@@ -1155,28 +1155,28 @@
       </c>
       <c r="U10" s="8"/>
     </row>
-    <row r="11" spans="1:21" ht="23.25">
+    <row r="11" spans="1:21" ht="23.4">
       <c r="B11" s="9"/>
       <c r="E11" s="8" t="s">
         <v>2</v>
       </c>
       <c r="U11" s="8"/>
     </row>
-    <row r="12" spans="1:21" ht="23.25">
+    <row r="12" spans="1:21" ht="23.4">
       <c r="E12" s="8" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:21" ht="23.25">
+    <row r="13" spans="1:21" ht="23.4">
       <c r="B13" s="9"/>
       <c r="C13" s="3"/>
     </row>
-    <row r="14" spans="1:21" ht="26.25">
+    <row r="14" spans="1:21" ht="25.8">
       <c r="A14" s="10" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:21" ht="26.25">
+    <row r="16" spans="1:21" ht="25.8">
       <c r="A16" s="2" t="s">
         <v>15</v>
       </c>
@@ -1197,7 +1197,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="1:14" ht="23.25">
+    <row r="17" spans="1:14" ht="23.4">
       <c r="I17" s="8" t="s">
         <v>18</v>
       </c>
@@ -1205,12 +1205,12 @@
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="1:14" ht="23.25">
+    <row r="18" spans="1:14" ht="23.4">
       <c r="I18" s="8" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:14" ht="26.25">
+    <row r="20" spans="1:14" ht="25.8">
       <c r="A20" s="2" t="s">
         <v>12</v>
       </c>
@@ -1221,7 +1221,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="21" spans="1:14" ht="23.25">
+    <row r="21" spans="1:14" ht="23.4">
       <c r="C21" s="8" t="s">
         <v>24</v>
       </c>
@@ -1236,22 +1236,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:N106"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N107" sqref="N107"/>
+    <sheetView tabSelected="1" topLeftCell="A72" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="F93" sqref="F93"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="43.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="43.88671875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="19.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:12" ht="28.5">
+    <row r="2" spans="2:12" ht="28.8">
       <c r="B2" s="11" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="4" spans="2:12" ht="26.25">
+    <row r="4" spans="2:12" ht="25.8">
       <c r="B4" s="15" t="s">
         <v>25</v>
       </c>
@@ -1278,7 +1278,7 @@
       <c r="K4" s="17"/>
       <c r="L4" s="17"/>
     </row>
-    <row r="5" spans="2:12" ht="18.75">
+    <row r="5" spans="2:12" ht="18">
       <c r="B5" s="27" t="s">
         <v>30</v>
       </c>
@@ -1305,7 +1305,7 @@
       </c>
       <c r="L5" s="23"/>
     </row>
-    <row r="6" spans="2:12" ht="18.75">
+    <row r="6" spans="2:12" ht="18">
       <c r="B6" s="27" t="s">
         <v>149</v>
       </c>
@@ -1332,7 +1332,7 @@
       </c>
       <c r="L6" s="23"/>
     </row>
-    <row r="7" spans="2:12" ht="18.75">
+    <row r="7" spans="2:12" ht="18">
       <c r="B7" s="27" t="s">
         <v>150</v>
       </c>
@@ -1359,7 +1359,7 @@
       </c>
       <c r="L7" s="23"/>
     </row>
-    <row r="8" spans="2:12" ht="18.75">
+    <row r="8" spans="2:12" ht="18">
       <c r="B8" s="27" t="s">
         <v>166</v>
       </c>
@@ -1386,7 +1386,7 @@
       </c>
       <c r="L8" s="23"/>
     </row>
-    <row r="9" spans="2:12" ht="18.75">
+    <row r="9" spans="2:12" ht="18">
       <c r="B9" s="27" t="s">
         <v>88</v>
       </c>
@@ -1413,7 +1413,7 @@
       </c>
       <c r="L9" s="23"/>
     </row>
-    <row r="10" spans="2:12" ht="18.75">
+    <row r="10" spans="2:12" ht="18">
       <c r="B10" s="27" t="s">
         <v>130</v>
       </c>
@@ -1440,7 +1440,7 @@
       </c>
       <c r="L10" s="23"/>
     </row>
-    <row r="11" spans="2:12" ht="18.75">
+    <row r="11" spans="2:12" ht="18">
       <c r="B11" s="27" t="s">
         <v>41</v>
       </c>
@@ -1467,7 +1467,7 @@
       </c>
       <c r="L11" s="23"/>
     </row>
-    <row r="12" spans="2:12" ht="18.75">
+    <row r="12" spans="2:12" ht="18">
       <c r="B12" s="27" t="s">
         <v>120</v>
       </c>
@@ -1494,7 +1494,7 @@
       </c>
       <c r="L12" s="23"/>
     </row>
-    <row r="13" spans="2:12" ht="18.75">
+    <row r="13" spans="2:12" ht="18">
       <c r="B13" s="27" t="s">
         <v>44</v>
       </c>
@@ -1521,7 +1521,7 @@
       </c>
       <c r="L13" s="23"/>
     </row>
-    <row r="14" spans="2:12" ht="18.75">
+    <row r="14" spans="2:12" ht="18">
       <c r="B14" s="27" t="s">
         <v>108</v>
       </c>
@@ -1548,7 +1548,7 @@
       </c>
       <c r="L14" s="20"/>
     </row>
-    <row r="15" spans="2:12" ht="18.75">
+    <row r="15" spans="2:12" ht="18">
       <c r="B15" s="27" t="s">
         <v>151</v>
       </c>
@@ -1575,7 +1575,7 @@
       </c>
       <c r="L15" s="20"/>
     </row>
-    <row r="16" spans="2:12" ht="18.75">
+    <row r="16" spans="2:12" ht="18">
       <c r="B16" s="27" t="s">
         <v>153</v>
       </c>
@@ -1602,7 +1602,7 @@
       </c>
       <c r="L16" s="20"/>
     </row>
-    <row r="17" spans="2:12" ht="18.75">
+    <row r="17" spans="2:12" ht="18">
       <c r="B17" s="27" t="s">
         <v>154</v>
       </c>
@@ -1629,12 +1629,12 @@
       </c>
       <c r="L17" s="20"/>
     </row>
-    <row r="19" spans="2:12" ht="31.5">
+    <row r="19" spans="2:12" ht="31.2">
       <c r="B19" s="1" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="21" spans="2:12" ht="26.25">
+    <row r="21" spans="2:12" ht="25.8">
       <c r="B21" s="13" t="s">
         <v>25</v>
       </c>
@@ -1661,7 +1661,7 @@
       <c r="K21" s="21"/>
       <c r="L21" s="21"/>
     </row>
-    <row r="22" spans="2:12" ht="18.75">
+    <row r="22" spans="2:12" ht="18">
       <c r="B22" s="23" t="s">
         <v>30</v>
       </c>
@@ -1688,7 +1688,7 @@
       <c r="K22" s="23"/>
       <c r="L22" s="23"/>
     </row>
-    <row r="23" spans="2:12" ht="18.75">
+    <row r="23" spans="2:12" ht="18">
       <c r="B23" s="23" t="s">
         <v>50</v>
       </c>
@@ -1715,7 +1715,7 @@
       <c r="K23" s="23"/>
       <c r="L23" s="23"/>
     </row>
-    <row r="24" spans="2:12" ht="18.75">
+    <row r="24" spans="2:12" ht="18">
       <c r="B24" s="23" t="s">
         <v>33</v>
       </c>
@@ -1742,7 +1742,7 @@
       <c r="K24" s="23"/>
       <c r="L24" s="23"/>
     </row>
-    <row r="25" spans="2:12" ht="18.75">
+    <row r="25" spans="2:12" ht="18">
       <c r="B25" s="23" t="s">
         <v>84</v>
       </c>
@@ -1769,7 +1769,7 @@
       <c r="K25" s="23"/>
       <c r="L25" s="23"/>
     </row>
-    <row r="26" spans="2:12" ht="18.75">
+    <row r="26" spans="2:12" ht="18">
       <c r="B26" s="23" t="s">
         <v>28</v>
       </c>
@@ -1796,7 +1796,7 @@
       <c r="K26" s="23"/>
       <c r="L26" s="23"/>
     </row>
-    <row r="27" spans="2:12" ht="18.75">
+    <row r="27" spans="2:12" ht="18">
       <c r="B27" s="23" t="s">
         <v>61</v>
       </c>
@@ -1823,7 +1823,7 @@
       <c r="K27" s="23"/>
       <c r="L27" s="23"/>
     </row>
-    <row r="28" spans="2:12" ht="18.75">
+    <row r="28" spans="2:12" ht="18">
       <c r="B28" s="23" t="s">
         <v>64</v>
       </c>
@@ -1850,7 +1850,7 @@
       <c r="K28" s="23"/>
       <c r="L28" s="23"/>
     </row>
-    <row r="29" spans="2:12" ht="18.75">
+    <row r="29" spans="2:12" ht="18">
       <c r="B29" s="23" t="s">
         <v>174</v>
       </c>
@@ -1877,7 +1877,7 @@
       <c r="K29" s="23"/>
       <c r="L29" s="23"/>
     </row>
-    <row r="30" spans="2:12" ht="18.75">
+    <row r="30" spans="2:12" ht="18">
       <c r="B30" s="23" t="s">
         <v>67</v>
       </c>
@@ -1904,7 +1904,7 @@
       <c r="K30" s="23"/>
       <c r="L30" s="23"/>
     </row>
-    <row r="31" spans="2:12" ht="18.75">
+    <row r="31" spans="2:12" ht="18">
       <c r="B31" s="23" t="s">
         <v>114</v>
       </c>
@@ -1931,7 +1931,7 @@
       <c r="K31" s="23"/>
       <c r="L31" s="23"/>
     </row>
-    <row r="32" spans="2:12" ht="18.75">
+    <row r="32" spans="2:12" ht="18">
       <c r="B32" s="23" t="s">
         <v>141</v>
       </c>
@@ -1958,7 +1958,7 @@
       <c r="K32" s="23"/>
       <c r="L32" s="23"/>
     </row>
-    <row r="33" spans="2:14" ht="18.75">
+    <row r="33" spans="2:14" ht="18">
       <c r="B33" s="23" t="s">
         <v>179</v>
       </c>
@@ -1985,7 +1985,7 @@
       <c r="K33" s="23"/>
       <c r="L33" s="23"/>
     </row>
-    <row r="34" spans="2:14" ht="18.75">
+    <row r="34" spans="2:14" ht="18">
       <c r="B34" s="23" t="s">
         <v>152</v>
       </c>
@@ -2012,7 +2012,7 @@
       <c r="K34" s="23"/>
       <c r="L34" s="23"/>
     </row>
-    <row r="35" spans="2:14" ht="18.75">
+    <row r="35" spans="2:14" ht="18">
       <c r="B35" s="23" t="s">
         <v>172</v>
       </c>
@@ -2039,7 +2039,7 @@
       <c r="K35" s="23"/>
       <c r="L35" s="23"/>
     </row>
-    <row r="37" spans="2:14" ht="31.5">
+    <row r="37" spans="2:14" ht="31.2">
       <c r="B37" s="1" t="s">
         <v>92</v>
       </c>
@@ -2049,7 +2049,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="39" spans="2:14" ht="26.25">
+    <row r="39" spans="2:14" ht="25.8">
       <c r="B39" s="13" t="s">
         <v>69</v>
       </c>
@@ -2076,7 +2076,7 @@
       <c r="K39" s="21"/>
       <c r="L39" s="18"/>
     </row>
-    <row r="40" spans="2:14" ht="18.75">
+    <row r="40" spans="2:14" ht="18">
       <c r="B40" s="23" t="s">
         <v>70</v>
       </c>
@@ -2103,7 +2103,7 @@
       <c r="K40" s="23"/>
       <c r="L40" s="23"/>
     </row>
-    <row r="41" spans="2:14" ht="18.75">
+    <row r="41" spans="2:14" ht="18">
       <c r="B41" s="23" t="s">
         <v>80</v>
       </c>
@@ -2133,7 +2133,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="42" spans="2:14" ht="18.75">
+    <row r="42" spans="2:14" ht="18">
       <c r="B42" s="23" t="s">
         <v>67</v>
       </c>
@@ -2160,7 +2160,7 @@
       <c r="K42" s="23"/>
       <c r="L42" s="23"/>
     </row>
-    <row r="43" spans="2:14" ht="18.75">
+    <row r="43" spans="2:14" ht="18">
       <c r="B43" s="23" t="s">
         <v>122</v>
       </c>
@@ -2187,7 +2187,7 @@
       <c r="K43" s="23"/>
       <c r="L43" s="23"/>
     </row>
-    <row r="44" spans="2:14" ht="18.75">
+    <row r="44" spans="2:14" ht="18">
       <c r="B44" s="23" t="s">
         <v>85</v>
       </c>
@@ -2214,7 +2214,7 @@
       <c r="K44" s="23"/>
       <c r="L44" s="23"/>
     </row>
-    <row r="45" spans="2:14" ht="18.75">
+    <row r="45" spans="2:14" ht="18">
       <c r="B45" s="23" t="s">
         <v>161</v>
       </c>
@@ -2241,7 +2241,7 @@
       <c r="K45" s="23"/>
       <c r="L45" s="23"/>
     </row>
-    <row r="46" spans="2:14" ht="18.75">
+    <row r="46" spans="2:14" ht="18">
       <c r="B46" s="23" t="s">
         <v>95</v>
       </c>
@@ -2268,7 +2268,7 @@
       <c r="K46" s="23"/>
       <c r="L46" s="23"/>
     </row>
-    <row r="47" spans="2:14" ht="18.75">
+    <row r="47" spans="2:14" ht="18">
       <c r="B47" s="23" t="s">
         <v>98</v>
       </c>
@@ -2295,7 +2295,7 @@
       <c r="K47" s="23"/>
       <c r="L47" s="23"/>
     </row>
-    <row r="48" spans="2:14" ht="18.75">
+    <row r="48" spans="2:14" ht="18">
       <c r="B48" s="23" t="s">
         <v>175</v>
       </c>
@@ -2310,7 +2310,7 @@
       <c r="K48" s="23"/>
       <c r="L48" s="23"/>
     </row>
-    <row r="49" spans="2:12" ht="18.75">
+    <row r="49" spans="2:12" ht="18">
       <c r="B49" s="23" t="s">
         <v>118</v>
       </c>
@@ -2337,7 +2337,7 @@
       <c r="K49" s="23"/>
       <c r="L49" s="23"/>
     </row>
-    <row r="50" spans="2:12" ht="18.75">
+    <row r="50" spans="2:12" ht="18">
       <c r="B50" s="23" t="s">
         <v>98</v>
       </c>
@@ -2366,7 +2366,7 @@
       <c r="K50" s="23"/>
       <c r="L50" s="23"/>
     </row>
-    <row r="51" spans="2:12" ht="18.75">
+    <row r="51" spans="2:12" ht="18">
       <c r="B51" s="23" t="s">
         <v>144</v>
       </c>
@@ -2393,7 +2393,7 @@
       <c r="K51" s="23"/>
       <c r="L51" s="23"/>
     </row>
-    <row r="52" spans="2:12" ht="18.75">
+    <row r="52" spans="2:12" ht="18">
       <c r="B52" s="23" t="s">
         <v>116</v>
       </c>
@@ -2420,12 +2420,12 @@
       <c r="K52" s="20"/>
       <c r="L52" s="20"/>
     </row>
-    <row r="54" spans="2:12" ht="28.5">
+    <row r="54" spans="2:12" ht="28.8">
       <c r="B54" s="11" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="56" spans="2:12" ht="26.25">
+    <row r="56" spans="2:12" ht="25.8">
       <c r="B56" s="13" t="s">
         <v>25</v>
       </c>
@@ -2452,7 +2452,7 @@
       <c r="K56" s="13"/>
       <c r="L56" s="14"/>
     </row>
-    <row r="57" spans="2:12" ht="18.75">
+    <row r="57" spans="2:12" ht="18">
       <c r="B57" s="23" t="s">
         <v>30</v>
       </c>
@@ -2479,7 +2479,7 @@
       <c r="K57" s="23"/>
       <c r="L57" s="23"/>
     </row>
-    <row r="58" spans="2:12" ht="18.75">
+    <row r="58" spans="2:12" ht="18">
       <c r="B58" s="23" t="s">
         <v>80</v>
       </c>
@@ -2506,7 +2506,7 @@
       <c r="K58" s="23"/>
       <c r="L58" s="23"/>
     </row>
-    <row r="59" spans="2:12" ht="18.75">
+    <row r="59" spans="2:12" ht="18">
       <c r="B59" s="23" t="s">
         <v>85</v>
       </c>
@@ -2533,7 +2533,7 @@
       <c r="K59" s="23"/>
       <c r="L59" s="23"/>
     </row>
-    <row r="60" spans="2:12" ht="18.75">
+    <row r="60" spans="2:12" ht="18">
       <c r="B60" s="23" t="s">
         <v>174</v>
       </c>
@@ -2560,7 +2560,7 @@
       <c r="K60" s="23"/>
       <c r="L60" s="23"/>
     </row>
-    <row r="61" spans="2:12" ht="18.75">
+    <row r="61" spans="2:12" ht="18">
       <c r="B61" s="23" t="s">
         <v>67</v>
       </c>
@@ -2590,12 +2590,12 @@
     <row r="62" spans="2:12">
       <c r="B62" s="12"/>
     </row>
-    <row r="63" spans="2:12" ht="31.5">
+    <row r="63" spans="2:12" ht="31.2">
       <c r="B63" s="1" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="65" spans="2:12" ht="26.25">
+    <row r="65" spans="2:12" ht="25.8">
       <c r="B65" s="13" t="s">
         <v>69</v>
       </c>
@@ -2622,7 +2622,7 @@
       <c r="K65" s="13"/>
       <c r="L65" s="18"/>
     </row>
-    <row r="66" spans="2:12" ht="18.75">
+    <row r="66" spans="2:12" ht="18">
       <c r="B66" s="23" t="s">
         <v>30</v>
       </c>
@@ -2649,7 +2649,7 @@
       <c r="K66" s="23"/>
       <c r="L66" s="23"/>
     </row>
-    <row r="67" spans="2:12" ht="18.75">
+    <row r="67" spans="2:12" ht="18">
       <c r="B67" s="23" t="s">
         <v>33</v>
       </c>
@@ -2676,12 +2676,12 @@
       <c r="K67" s="23"/>
       <c r="L67" s="23"/>
     </row>
-    <row r="69" spans="2:12" ht="31.5">
+    <row r="69" spans="2:12" ht="31.2">
       <c r="B69" s="1" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="71" spans="2:12" ht="26.25">
+    <row r="71" spans="2:12" ht="25.8">
       <c r="B71" s="13" t="s">
         <v>25</v>
       </c>
@@ -2708,7 +2708,7 @@
       <c r="K71" s="13"/>
       <c r="L71" s="21"/>
     </row>
-    <row r="72" spans="2:12" ht="18.75">
+    <row r="72" spans="2:12" ht="18">
       <c r="B72" s="23" t="s">
         <v>30</v>
       </c>
@@ -2735,7 +2735,7 @@
       <c r="K72" s="23"/>
       <c r="L72" s="23"/>
     </row>
-    <row r="73" spans="2:12" ht="18.75">
+    <row r="73" spans="2:12" ht="18">
       <c r="B73" s="27" t="s">
         <v>149</v>
       </c>
@@ -2762,7 +2762,7 @@
       <c r="K73" s="23"/>
       <c r="L73" s="23"/>
     </row>
-    <row r="74" spans="2:12" ht="18.75">
+    <row r="74" spans="2:12" ht="18">
       <c r="B74" s="23" t="s">
         <v>150</v>
       </c>
@@ -2789,7 +2789,7 @@
       <c r="K74" s="23"/>
       <c r="L74" s="23"/>
     </row>
-    <row r="75" spans="2:12" ht="18.75">
+    <row r="75" spans="2:12" ht="18">
       <c r="B75" s="23" t="s">
         <v>102</v>
       </c>
@@ -2816,7 +2816,7 @@
       <c r="K75" s="23"/>
       <c r="L75" s="23"/>
     </row>
-    <row r="76" spans="2:12" ht="18.75">
+    <row r="76" spans="2:12" ht="18">
       <c r="B76" s="23" t="s">
         <v>88</v>
       </c>
@@ -2843,7 +2843,7 @@
       <c r="K76" s="23"/>
       <c r="L76" s="23"/>
     </row>
-    <row r="77" spans="2:12" ht="18.75">
+    <row r="77" spans="2:12" ht="18">
       <c r="B77" s="23" t="s">
         <v>174</v>
       </c>
@@ -2870,7 +2870,7 @@
       <c r="K77" s="23"/>
       <c r="L77" s="23"/>
     </row>
-    <row r="78" spans="2:12" ht="18.75">
+    <row r="78" spans="2:12" ht="18">
       <c r="B78" s="23" t="s">
         <v>114</v>
       </c>
@@ -2897,7 +2897,7 @@
       <c r="K78" s="23"/>
       <c r="L78" s="23"/>
     </row>
-    <row r="79" spans="2:12" ht="18.75">
+    <row r="79" spans="2:12" ht="18">
       <c r="B79" s="23" t="s">
         <v>36</v>
       </c>
@@ -2924,12 +2924,12 @@
       <c r="K79" s="20"/>
       <c r="L79" s="20"/>
     </row>
-    <row r="81" spans="2:12" ht="31.5">
+    <row r="81" spans="2:12" ht="31.2">
       <c r="B81" s="1" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="83" spans="2:12" ht="26.25">
+    <row r="83" spans="2:12" ht="25.8">
       <c r="B83" s="13" t="s">
         <v>25</v>
       </c>
@@ -2956,7 +2956,7 @@
       <c r="K83" s="13"/>
       <c r="L83" s="21"/>
     </row>
-    <row r="84" spans="2:12" ht="18.75">
+    <row r="84" spans="2:12" ht="18">
       <c r="B84" s="23" t="s">
         <v>30</v>
       </c>
@@ -2983,7 +2983,7 @@
       <c r="K84" s="23"/>
       <c r="L84" s="23"/>
     </row>
-    <row r="85" spans="2:12" ht="18.75">
+    <row r="85" spans="2:12" ht="18">
       <c r="B85" s="23" t="s">
         <v>33</v>
       </c>
@@ -3010,12 +3010,12 @@
       <c r="K85" s="23"/>
       <c r="L85" s="23"/>
     </row>
-    <row r="87" spans="2:12" ht="31.5">
+    <row r="87" spans="2:12" ht="31.2">
       <c r="B87" s="1" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="89" spans="2:12" ht="26.25">
+    <row r="89" spans="2:12" ht="25.8">
       <c r="B89" s="13" t="s">
         <v>69</v>
       </c>
@@ -3042,7 +3042,7 @@
       <c r="K89" s="13"/>
       <c r="L89" s="13"/>
     </row>
-    <row r="90" spans="2:12" ht="18.75">
+    <row r="90" spans="2:12" ht="18">
       <c r="B90" s="23" t="s">
         <v>30</v>
       </c>
@@ -3069,7 +3069,7 @@
       <c r="K90" s="23"/>
       <c r="L90" s="23"/>
     </row>
-    <row r="91" spans="2:12" ht="18.75">
+    <row r="91" spans="2:12" ht="18">
       <c r="B91" s="23" t="s">
         <v>33</v>
       </c>
@@ -3096,7 +3096,7 @@
       <c r="K91" s="23"/>
       <c r="L91" s="23"/>
     </row>
-    <row r="92" spans="2:12" ht="18.75">
+    <row r="92" spans="2:12" ht="18">
       <c r="B92" s="23" t="s">
         <v>135</v>
       </c>
@@ -3123,7 +3123,7 @@
       <c r="K92" s="23"/>
       <c r="L92" s="23"/>
     </row>
-    <row r="93" spans="2:12" ht="18.75">
+    <row r="93" spans="2:12" ht="18">
       <c r="B93" s="23" t="s">
         <v>137</v>
       </c>
@@ -3150,12 +3150,12 @@
       <c r="K93" s="23"/>
       <c r="L93" s="23"/>
     </row>
-    <row r="95" spans="2:12" ht="31.5">
+    <row r="95" spans="2:12" ht="31.2">
       <c r="B95" s="1" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="97" spans="2:12" ht="26.25">
+    <row r="97" spans="2:12" ht="25.8">
       <c r="B97" s="13" t="s">
         <v>69</v>
       </c>
@@ -3182,7 +3182,7 @@
       <c r="K97" s="13"/>
       <c r="L97" s="13"/>
     </row>
-    <row r="98" spans="2:12" ht="18.75">
+    <row r="98" spans="2:12" ht="18">
       <c r="B98" s="23" t="s">
         <v>30</v>
       </c>
@@ -3209,7 +3209,7 @@
       <c r="K98" s="23"/>
       <c r="L98" s="23"/>
     </row>
-    <row r="99" spans="2:12" ht="18.75">
+    <row r="99" spans="2:12" ht="18">
       <c r="B99" s="23" t="s">
         <v>33</v>
       </c>
@@ -3236,12 +3236,12 @@
       <c r="K99" s="23"/>
       <c r="L99" s="23"/>
     </row>
-    <row r="101" spans="2:12" ht="31.5">
+    <row r="101" spans="2:12" ht="31.2">
       <c r="B101" s="1" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="103" spans="2:12" ht="26.25">
+    <row r="103" spans="2:12" ht="25.8">
       <c r="B103" s="13" t="s">
         <v>69</v>
       </c>
@@ -3268,7 +3268,7 @@
       <c r="K103" s="13"/>
       <c r="L103" s="13"/>
     </row>
-    <row r="104" spans="2:12" ht="18.75">
+    <row r="104" spans="2:12" ht="18">
       <c r="B104" s="23" t="s">
         <v>30</v>
       </c>
@@ -3295,7 +3295,7 @@
       <c r="K104" s="23"/>
       <c r="L104" s="23"/>
     </row>
-    <row r="105" spans="2:12" ht="18.75">
+    <row r="105" spans="2:12" ht="18">
       <c r="B105" s="23" t="s">
         <v>181</v>
       </c>
@@ -3322,7 +3322,7 @@
       <c r="K105" s="23"/>
       <c r="L105" s="23"/>
     </row>
-    <row r="106" spans="2:12" ht="18.75">
+    <row r="106" spans="2:12" ht="18">
       <c r="B106" s="23" t="s">
         <v>85</v>
       </c>
@@ -3363,7 +3363,7 @@
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="4" spans="1:5">
       <c r="E4" t="s">

</xml_diff>